<commit_message>
Adding verification scripts/files for CCDP test case category 3
</commit_message>
<xml_diff>
--- a/docs/packages/CCDP/test_cases/CCDP Test Cases.xlsx
+++ b/docs/packages/CCDP/test_cases/CCDP Test Cases.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="8205"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="8205" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Category 1 Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Category 2 Cruise Tests" sheetId="2" r:id="rId2"/>
     <sheet name="Category 2 DVM Tests" sheetId="3" r:id="rId3"/>
+    <sheet name="Category 3 Cruise Tests" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="92">
   <si>
     <t>HA1007</t>
   </si>
@@ -301,6 +302,123 @@
 The generate filtered option query was NOT successful
 ORA-20614: The P_MAIN_QUERY parameter is blank
 completed test case for ORA-20614</t>
+  </si>
+  <si>
+    <t>Reference Table Name</t>
+  </si>
+  <si>
+    <t>CCD_REG_ECOSYSTEMS</t>
+  </si>
+  <si>
+    <t>{
+"options":[
+{
+"OPTION_VALUE":"Eastern Tropical Pacific"
+,"OPTION_ID":5
+}
+,{
+"OPTION_VALUE":"Great Lakes"
+,"OPTION_ID":6
+}
+,{
+"OPTION_VALUE":"Northeast Shelf"
+,"OPTION_ID":9
+}
+,{
+"OPTION_VALUE":"Pacific Islands Ecosystem Complex"
+,"OPTION_ID":10
+}
+,{
+"OPTION_VALUE":"Southeast Shelf"
+,"OPTION_ID":11
+}
+]
+}</t>
+  </si>
+  <si>
+    <t>Filtered reference table records for:
+OES0410 that is associated with the Gulf of California</t>
+  </si>
+  <si>
+    <t>Filtered reference table records for:
+RL-17-05 Leg 1
+including two additional regional ecosystems (Great Lakes, Southeast Shelf)</t>
+  </si>
+  <si>
+    <t>{
+"options":[
+{
+"OPTION_VALUE":"Alaska Ecosystem Complex"
+,"OPTION_ID":1
+}
+,{
+"OPTION_VALUE":"Antarctica"
+,"OPTION_ID":2
+}
+,{
+"OPTION_VALUE":"California Current"
+,"OPTION_ID":3
+}
+,{
+"OPTION_VALUE":"Caribbean Sea"
+,"OPTION_ID":4
+}
+,{
+"OPTION_VALUE":"Eastern Tropical Pacific"
+,"OPTION_ID":5
+}
+,{
+"OPTION_VALUE":"Great Lakes"
+,"OPTION_ID":6
+}
+,{
+"OPTION_VALUE":"Gulf of California"
+,"OPTION_ID":7
+}
+,{
+"OPTION_VALUE":"Gulf of Mexico"
+,"OPTION_ID":8
+}
+,{
+"OPTION_VALUE":"Northeast Shelf"
+,"OPTION_ID":9
+}
+,{
+"OPTION_VALUE":"Pacific Islands Ecosystem Complex"
+,"OPTION_ID":10
+}
+,{
+"OPTION_VALUE":"Southeast Shelf"
+,"OPTION_ID":11
+}
+]
+}</t>
+  </si>
+  <si>
+    <t>Unfiltered reference table records for:
+OES0410</t>
+  </si>
+  <si>
+    <t>{
+"options":[
+{
+"OPTION_VALUE":"Eastern Tropical Pacific"
+,"OPTION_ID":5
+}
+,{
+"OPTION_VALUE":"Gulf of California"
+,"OPTION_ID":7
+}
+,{
+"OPTION_VALUE":"Northeast Shelf"
+,"OPTION_ID":9
+}
+,{
+"OPTION_VALUE":"Pacific Islands Ecosystem Complex"
+,"OPTION_ID":10
+}
+]
+}</t>
   </si>
 </sst>
 </file>
@@ -647,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1789,4 +1907,69 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="86.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="360" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="300" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated CCD_CRUISE_PKG.UPDATE_FIL_SHUTTLE_OPTIONS_SP to add a parameter to output to DBMS_OUTPUT.PUT_LINE for debugging purposes
</commit_message>
<xml_diff>
--- a/docs/packages/CCDP/test_cases/CCDP Test Cases.xlsx
+++ b/docs/packages/CCDP/test_cases/CCDP Test Cases.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="117">
   <si>
     <t>HA1007</t>
   </si>
@@ -419,6 +419,402 @@
 }
 ]
 }</t>
+  </si>
+  <si>
+    <t>CCD_EXP_SPP_CATS</t>
+  </si>
+  <si>
+    <t>Filtered reference table records for:
+TC9909
+with additional records: 
+Microbes
+Sea Grass</t>
+  </si>
+  <si>
+    <t>{
+"options":[
+{
+"OPTION_VALUE":"Algae"
+,"OPTION_ID":1
+}
+,{
+"OPTION_VALUE":"Coral-Hermatypic Stony Coral"
+,"OPTION_ID":3
+}
+,{
+"OPTION_VALUE":"Coral-Mesophotic Hermatypic Coral"
+,"OPTION_ID":5
+}
+,{
+"OPTION_VALUE":"Coral-Octocoral"
+,"OPTION_ID":6
+}
+,{
+"OPTION_VALUE":"Coral-Shallow Water Coral"
+,"OPTION_ID":7
+}
+,{
+"OPTION_VALUE":"Crustaceans"
+,"OPTION_ID":8
+}
+,{
+"OPTION_VALUE":"Fish-General"
+,"OPTION_ID":9
+}
+,{
+"OPTION_VALUE":"Fishes-Benthic Fish"
+,"OPTION_ID":10
+}
+,{
+"OPTION_VALUE":"Fishes-Pelagic Fish"
+,"OPTION_ID":12
+}
+,{
+"OPTION_VALUE":"Fishes-Reef Fish"
+,"OPTION_ID":13
+}
+,{
+"OPTION_VALUE":"Fishes-Shark"
+,"OPTION_ID":14
+}
+,{
+"OPTION_VALUE":"Invertebrate-Benthic"
+,"OPTION_ID":16
+}
+,{
+"OPTION_VALUE":"Invertebrate-General"
+,"OPTION_ID":17
+}
+,{
+"OPTION_VALUE":"Microbes"
+,"OPTION_ID":20
+}
+,{
+"OPTION_VALUE":"Sea Grass"
+,"OPTION_ID":23
+}
+,{
+"OPTION_VALUE":"Sea Turtle"
+,"OPTION_ID":24
+}
+]
+}</t>
+  </si>
+  <si>
+    <t>Unfiltered reference table records for:
+SE-17-07</t>
+  </si>
+  <si>
+    <t>{
+"options":[
+{
+"OPTION_VALUE":"Algae"
+,"OPTION_ID":1
+}
+,{
+"OPTION_VALUE":"Coral-Deep Water Coral"
+,"OPTION_ID":2
+}
+,{
+"OPTION_VALUE":"Coral-Hermatypic Stony Coral"
+,"OPTION_ID":3
+}
+,{
+"OPTION_VALUE":"Coral-Hydrocoral"
+,"OPTION_ID":4
+}
+,{
+"OPTION_VALUE":"Coral-Mesophotic Hermatypic Coral"
+,"OPTION_ID":5
+}
+,{
+"OPTION_VALUE":"Coral-Octocoral"
+,"OPTION_ID":6
+}
+,{
+"OPTION_VALUE":"Coral-Shallow Water Coral"
+,"OPTION_ID":7
+}
+,{
+"OPTION_VALUE":"Crustaceans"
+,"OPTION_ID":8
+}
+,{
+"OPTION_VALUE":"Fish-General"
+,"OPTION_ID":9
+}
+,{
+"OPTION_VALUE":"Fishes-Benthic Fish"
+,"OPTION_ID":10
+}
+,{
+"OPTION_VALUE":"Fishes-Larval Reef Fish"
+,"OPTION_ID":11
+}
+,{
+"OPTION_VALUE":"Fishes-Pelagic Fish"
+,"OPTION_ID":12
+}
+,{
+"OPTION_VALUE":"Fishes-Reef Fish"
+,"OPTION_ID":13
+}
+,{
+"OPTION_VALUE":"Fishes-Shark"
+,"OPTION_ID":14
+}
+,{
+"OPTION_VALUE":"Ichthyoplankton"
+,"OPTION_ID":15
+}
+,{
+"OPTION_VALUE":"Invertebrate-Benthic"
+,"OPTION_ID":16
+}
+,{
+"OPTION_VALUE":"Invertebrate-General"
+,"OPTION_ID":17
+}
+,{
+"OPTION_VALUE":"Invertebrate-Pelagic"
+,"OPTION_ID":18
+}
+,{
+"OPTION_VALUE":"Marine Mammal"
+,"OPTION_ID":19
+}
+,{
+"OPTION_VALUE":"Microbes"
+,"OPTION_ID":20
+}
+,{
+"OPTION_VALUE":"Phytoplankton"
+,"OPTION_ID":21
+}
+,{
+"OPTION_VALUE":"Sea Bird"
+,"OPTION_ID":22
+}
+,{
+"OPTION_VALUE":"Sea Grass"
+,"OPTION_ID":23
+}
+,{
+"OPTION_VALUE":"Sea Turtle"
+,"OPTION_ID":24
+}
+,{
+"OPTION_VALUE":"Zooplankton"
+,"OPTION_ID":25
+}
+]
+}</t>
+  </si>
+  <si>
+    <t>Filtered reference table records for:
+HA1007
+associated with 
+Marine Mammal
+Sea Grass
+With extra options:
+Coral-Hydrocoral
+Microbes</t>
+  </si>
+  <si>
+    <t>{
+"options":[
+{
+"OPTION_VALUE":"Algae"
+,"OPTION_ID":1
+}
+,{
+"OPTION_VALUE":"Coral-Hermatypic Stony Coral"
+,"OPTION_ID":3
+}
+,{
+"OPTION_VALUE":"Coral-Hydrocoral"
+,"OPTION_ID":4
+}
+,{
+"OPTION_VALUE":"Coral-Mesophotic Hermatypic Coral"
+,"OPTION_ID":5
+}
+,{
+"OPTION_VALUE":"Coral-Octocoral"
+,"OPTION_ID":6
+}
+,{
+"OPTION_VALUE":"Coral-Shallow Water Coral"
+,"OPTION_ID":7
+}
+,{
+"OPTION_VALUE":"Crustaceans"
+,"OPTION_ID":8
+}
+,{
+"OPTION_VALUE":"Fish-General"
+,"OPTION_ID":9
+}
+,{
+"OPTION_VALUE":"Fishes-Benthic Fish"
+,"OPTION_ID":10
+}
+,{
+"OPTION_VALUE":"Fishes-Pelagic Fish"
+,"OPTION_ID":12
+}
+,{
+"OPTION_VALUE":"Fishes-Reef Fish"
+,"OPTION_ID":13
+}
+,{
+"OPTION_VALUE":"Fishes-Shark"
+,"OPTION_ID":14
+}
+,{
+"OPTION_VALUE":"Invertebrate-Benthic"
+,"OPTION_ID":16
+}
+,{
+"OPTION_VALUE":"Invertebrate-General"
+,"OPTION_ID":17
+}
+,{
+"OPTION_VALUE":"Marine Mammal"
+,"OPTION_ID":19
+}
+,{
+"OPTION_VALUE":"Microbes"
+,"OPTION_ID":20
+}
+,{
+"OPTION_VALUE":"Sea Grass"
+,"OPTION_ID":23
+}
+,{
+"OPTION_VALUE":"Sea Turtle"
+,"OPTION_ID":24
+}
+]
+}</t>
+  </si>
+  <si>
+    <t>Procedure/Function</t>
+  </si>
+  <si>
+    <t>CCD_CRUISE_PKG.UPDATE_FIL_SHUTTLE_OPTIONS_SP</t>
+  </si>
+  <si>
+    <t>CCD_CRUISE_PKG.GEN_FIL_OPTION_QUERY_FN</t>
+  </si>
+  <si>
+    <t>ESA target species main query is defined, query fragment is defined and some option IDs are included</t>
+  </si>
+  <si>
+    <t>CCD_TGT_SPP_ESA</t>
+  </si>
+  <si>
+    <t>regional ecosystem main query is defined, query fragment is defined and some option IDs are included</t>
+  </si>
+  <si>
+    <t>gear main query is defined, query fragment is defined and some option IDs are included</t>
+  </si>
+  <si>
+    <t>CCD_GEAR</t>
+  </si>
+  <si>
+    <t>CCD_TGT_SPP_MMPA</t>
+  </si>
+  <si>
+    <t>target MMPA species main query is defined but no query fragment is defined</t>
+  </si>
+  <si>
+    <t>target ESA species main query is defined but no query fragment is defined</t>
+  </si>
+  <si>
+    <t>SELECT
+    TGT_SPP_ESA_NAME OPTION_VALUE, TGT_SPP_ESA_ID OPTION_ID FROM CCD_TGT_SPP_ESA where TGT_SPP_ESA_ID IN
+    (
+        SELECT DISTINCT TGT_SPP_ESA_ID
+        FROM
+        (SELECT TGT_SPP_ESA_ID FROM CCD_TGT_SPP_ESA where (:P220_ESA_SHOW_FILT_LIST = ''Y'' AND APP_SHOW_OPT_YN = ''Y'') OR (:P220_ESA_SHOW_FILT_LIST IS NULL)
+        UNION
+        SELECT TGT_SPP_ESA_ID from CCD_CRUISE_SPP_ESA where cruise_id IN (:P220_CRUISE_ID, :P220_CRUISE_ID_COPY)
+  --query fragment goes here when defined:
+        )
+    )
+    ORDER BY UPPER(TGT_SPP_ESA_NAME)</t>
+  </si>
+  <si>
+    <t>SELECT
+    TGT_SPP_MMPA_NAME OPTION_VALUE, TGT_SPP_MMPA_ID OPTION_ID FROM CCD_TGT_SPP_MMPA where TGT_SPP_MMPA_ID IN
+    (
+        SELECT DISTINCT TGT_SPP_MMPA_ID
+        FROM
+        (SELECT TGT_SPP_MMPA_ID FROM CCD_TGT_SPP_MMPA where (:P220_MMPA_SHOW_FILT_LIST = ''Y'' AND APP_SHOW_OPT_YN = ''Y'') OR (:P220_MMPA_SHOW_FILT_LIST IS NULL)
+        UNION
+        SELECT TGT_SPP_MMPA_ID from CCD_CRUISE_SPP_MMPA where cruise_id IN (:P220_CRUISE_ID, :P220_CRUISE_ID_COPY)
+  --query fragment goes here when defined:
+        )
+    )
+    ORDER BY UPPER(TGT_SPP_MMPA_NAME)</t>
+  </si>
+  <si>
+    <t>MMPA target species main query is defined, query fragment is defined and no option IDs are included</t>
+  </si>
+  <si>
+    <t>SELECT
+    REG_ECOSYSTEM_NAME OPTION_VALUE, REG_ECOSYSTEM_ID OPTION_ID FROM CCD_REG_ECOSYSTEMS where REG_ECOSYSTEM_ID IN
+    (
+        SELECT DISTINCT REG_ECOSYSTEM_ID
+        FROM
+        (SELECT REG_ECOSYSTEM_ID FROM CCD_REG_ECOSYSTEMS where (:SHOW_FILT_LIST = ''Y'' AND APP_SHOW_OPT_YN = ''Y'') OR (:SHOW_FILT_LIST IS NULL)
+        UNION
+        SELECT REG_ECOSYSTEM_ID from CCD_LEG_ECOSYSTEMS where CRUISE_LEG_ID IN (:PK_ID)
+       UNION SELECT REG_ECOSYSTEM_ID FROM CCD_REG_ECOSYSTEMS where REG_ECOSYSTEM_ID IN (99, 1, 50))
+    )
+    ORDER BY UPPER(REG_ECOSYSTEM_NAME)</t>
+  </si>
+  <si>
+    <t>SELECT
+    GEAR_NAME OPTION_VALUE, GEAR_ID OPTION_ID FROM CCD_GEAR where GEAR_ID IN
+    (
+        SELECT DISTINCT GEAR_ID
+        FROM
+        (SELECT GEAR_ID FROM CCD_GEAR where (:SHOW_FILT_LIST = ''Y'' AND APP_SHOW_OPT_YN = ''Y'') OR (:SHOW_FILT_LIST IS NULL)
+        UNION
+        SELECT GEAR_ID from CCD_LEG_GEAR where CRUISE_LEG_ID IN (:PK_ID)
+        UNION SELECT GEAR_ID FROM CCD_GEAR where GEAR_ID IN (4, 20))
+    )
+    ORDER BY UPPER(GEAR_NAME)</t>
+  </si>
+  <si>
+    <t>SELECT
+    TGT_SPP_ESA_NAME OPTION_VALUE, TGT_SPP_ESA_ID OPTION_ID FROM CCD_TGT_SPP_ESA where TGT_SPP_ESA_ID IN
+    (
+        SELECT DISTINCT TGT_SPP_ESA_ID
+        FROM
+        (SELECT TGT_SPP_ESA_ID FROM CCD_TGT_SPP_ESA where (:SHOW_FILT_LIST = ''Y'' AND APP_SHOW_OPT_YN = ''Y'') OR (:SHOW_FILT_LIST IS NULL)
+        UNION
+        SELECT TGT_SPP_ESA_ID from CCD_CRUISE_SPP_ESA where cruise_id IN(:PK_ID)
+  --query fragment goes here when defined:
+        UNION SELECT TGT_SPP_ESA_ID FROM CCD_TGT_SPP_ESA where TGT_SPP_ESA_ID IN (20, 25, 14, 9))
+    )
+    ORDER BY UPPER(TGT_SPP_ESA_NAME)</t>
+  </si>
+  <si>
+    <t>SELECT
+    TGT_SPP_MMPA_NAME OPTION_VALUE, TGT_SPP_MMPA_ID OPTION_ID FROM CCD_TGT_SPP_MMPA where TGT_SPP_MMPA_ID IN
+    (
+        SELECT DISTINCT TGT_SPP_MMPA_ID
+        FROM
+        (SELECT TGT_SPP_MMPA_ID FROM CCD_TGT_SPP_MMPA where (:SHOW_FILT_LIST = ''Y'' AND APP_SHOW_OPT_YN = ''Y'') OR (:SHOW_FILT_LIST IS NULL)
+        UNION
+        SELECT TGT_SPP_MMPA_ID from CCD_CRUISE_SPP_MMPA where cruise_id IN(:PK_ID)
+  --query fragment goes here when defined:
+        )
+    )
+    ORDER BY UPPER(TGT_SPP_MMPA_NAME)</t>
   </si>
 </sst>
 </file>
@@ -448,12 +844,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -468,7 +870,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -482,6 +884,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1911,61 +2316,200 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="86.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.28515625" customWidth="1"/>
+    <col min="1" max="1" width="49.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="86.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="360" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="360" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="300" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="300" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="8" t="s">
         <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="285" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="285" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="240" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="285" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="300" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="285" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>